<commit_message>
Update Matiz de Pruebas Financiamiento y obligaciones  Consulta de Solicitudes  Perfil Capturador.xlsx
</commit_message>
<xml_diff>
--- a/SGCM/ENTREGABLES/Matiz de Pruebas Financiamiento y obligaciones  Consulta de Solicitudes  Perfil Capturador.xlsx
+++ b/SGCM/ENTREGABLES/Matiz de Pruebas Financiamiento y obligaciones  Consulta de Solicitudes  Perfil Capturador.xlsx
@@ -5731,13 +5731,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>11</xdr:col>
-          <xdr:colOff>1723582</xdr:colOff>
+          <xdr:colOff>1714057</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>886</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>12</xdr:col>
-          <xdr:colOff>313439</xdr:colOff>
+          <xdr:colOff>246764</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>200911</xdr:rowOff>
         </xdr:to>
@@ -5778,13 +5778,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>11</xdr:col>
-          <xdr:colOff>1723582</xdr:colOff>
+          <xdr:colOff>1714057</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>886</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>12</xdr:col>
-          <xdr:colOff>313439</xdr:colOff>
+          <xdr:colOff>246764</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>200911</xdr:rowOff>
         </xdr:to>
@@ -12416,9 +12416,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:N359"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
+      <selection pane="bottomLeft" activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -12933,7 +12933,7 @@
         <v>64</v>
       </c>
       <c r="G16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H16" s="20" t="s">
         <v>139</v>
@@ -12945,7 +12945,7 @@
         <v>39</v>
       </c>
       <c r="L16" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="M16" s="7" t="s">
         <v>140</v>
@@ -13056,7 +13056,7 @@
         <v>72</v>
       </c>
       <c r="G19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>142</v>
@@ -13069,7 +13069,7 @@
         <v>39</v>
       </c>
       <c r="L19" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="M19" s="7" t="s">
         <v>141</v>
@@ -14661,18 +14661,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="3088" r:id="rId10" name="Control 16">
+        <control shapeId="3090" r:id="rId10" name="Control 18">
           <controlPr defaultSize="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>11</xdr:col>
-                <xdr:colOff>1724025</xdr:colOff>
+                <xdr:colOff>1714500</xdr:colOff>
                 <xdr:row>9</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>12</xdr:col>
-                <xdr:colOff>314325</xdr:colOff>
+                <xdr:colOff>247650</xdr:colOff>
                 <xdr:row>9</xdr:row>
                 <xdr:rowOff>200025</xdr:rowOff>
               </to>
@@ -14681,23 +14681,23 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="3088" r:id="rId10" name="Control 16"/>
+        <control shapeId="3090" r:id="rId10" name="Control 18"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="3090" r:id="rId12" name="Control 18">
+        <control shapeId="3088" r:id="rId12" name="Control 16">
           <controlPr defaultSize="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>11</xdr:col>
-                <xdr:colOff>1724025</xdr:colOff>
+                <xdr:colOff>1714500</xdr:colOff>
                 <xdr:row>9</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>12</xdr:col>
-                <xdr:colOff>314325</xdr:colOff>
+                <xdr:colOff>247650</xdr:colOff>
                 <xdr:row>9</xdr:row>
                 <xdr:rowOff>200025</xdr:rowOff>
               </to>
@@ -14706,7 +14706,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="3090" r:id="rId12" name="Control 18"/>
+        <control shapeId="3088" r:id="rId12" name="Control 16"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>